<commit_message>
CARROT-v2, find the emptiest switch in the downstream
</commit_message>
<xml_diff>
--- a/CARROT/experiment/实验记录.xlsx
+++ b/CARROT/experiment/实验记录.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\AppData\Local\Temp\scp20084\home\pengzheng\hello-world\CARROT\experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\AppData\Local\Temp\scp55869\home\pengzheng\hello-world\CARROT\experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23892" windowHeight="10356" tabRatio="650" firstSheet="3" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23892" windowHeight="10356" tabRatio="650" firstSheet="6" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,13 +29,14 @@
     <sheet name="Sheet9" sheetId="15" r:id="rId15"/>
     <sheet name="CARROT-FIXED" sheetId="16" r:id="rId16"/>
     <sheet name="CARROT-VARIABLE" sheetId="17" r:id="rId17"/>
+    <sheet name="CARROT-VARIABLE (2)" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="134">
   <si>
     <t>程序：SplitCounter-v0.4</t>
   </si>
@@ -806,6 +807,45 @@
   <si>
     <t>Variable</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>program description: every time always find the first switch along the routing path to be the highest carry counter.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CARROT-Variable-v2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>least loaded first along the routing path avaliable, shorter flow</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>program description: every time always find the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> least loaded switch in the sownstream of the routing path </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to be the highest carry counter.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -5055,8 +5095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -5858,8 +5898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -6809,7 +6849,7 @@
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -7607,11 +7647,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -8389,6 +8432,726 @@
       <c r="V11">
         <f t="shared" si="4"/>
         <v>11070236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:L1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+      <c r="N1" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="86.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>28</v>
+      </c>
+      <c r="E3">
+        <f>D3</f>
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>50000</v>
+      </c>
+      <c r="H3">
+        <v>378866</v>
+      </c>
+      <c r="I3">
+        <v>89098</v>
+      </c>
+      <c r="J3">
+        <v>7577325</v>
+      </c>
+      <c r="K3">
+        <v>1981495</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L11" si="0">N3/J3</f>
+        <v>1.0664664640885801</v>
+      </c>
+      <c r="M3" s="4">
+        <v>24820432</v>
+      </c>
+      <c r="N3">
+        <v>8080963</v>
+      </c>
+      <c r="O3">
+        <f>N3/M3</f>
+        <v>0.32557704877981175</v>
+      </c>
+      <c r="P3">
+        <v>886441</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q11" si="1">P3/C3</f>
+        <v>44322.05</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R11" si="2">J3/1000/1000</f>
+        <v>7.5773250000000001</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S11" si="3">M3/1000/1000</f>
+        <v>24.820432</v>
+      </c>
+      <c r="T3">
+        <f>(S3-R3)/S3</f>
+        <v>0.69471421770579989</v>
+      </c>
+      <c r="U3">
+        <v>501506</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V11" si="4">U3*C3</f>
+        <v>10030120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E11" si="5">D4</f>
+        <v>29</v>
+      </c>
+      <c r="F4">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>80000</v>
+      </c>
+      <c r="L4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M4">
+        <v>42548423</v>
+      </c>
+      <c r="N4">
+        <v>12032580</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O11" si="6">N4/M4</f>
+        <v>0.28279732012629472</v>
+      </c>
+      <c r="P4">
+        <v>1467185</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>73359.25</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="3"/>
+        <v>42.548423</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T11" si="7">(S4-R4)/S4</f>
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>789235</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="4"/>
+        <v>15784700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>60000</v>
+      </c>
+      <c r="L5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5">
+        <v>30216782</v>
+      </c>
+      <c r="N5">
+        <v>9610585</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="6"/>
+        <v>0.31805454995174537</v>
+      </c>
+      <c r="P5">
+        <v>1041956</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>52097.8</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="3"/>
+        <v>30.216781999999998</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>568339</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="4"/>
+        <v>11366780</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="F6">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>30000</v>
+      </c>
+      <c r="L6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M6">
+        <v>24820348</v>
+      </c>
+      <c r="N6">
+        <v>8080963</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="6"/>
+        <v>0.32557815063672757</v>
+      </c>
+      <c r="P6">
+        <v>886441</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>24623.361111111109</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="3"/>
+        <v>24.820348000000003</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>302753</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="4"/>
+        <v>10899108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7">
+        <v>36</v>
+      </c>
+      <c r="D7">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="F7">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>50000</v>
+      </c>
+      <c r="L7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7">
+        <v>42548423</v>
+      </c>
+      <c r="N7">
+        <v>12032580</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="6"/>
+        <v>0.28279732012629472</v>
+      </c>
+      <c r="P7">
+        <v>1467185</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>40755.138888888891</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="3"/>
+        <v>42.548423</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>516086</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="4"/>
+        <v>18579096</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="F8">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>30000</v>
+      </c>
+      <c r="L8" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8">
+        <v>30216782</v>
+      </c>
+      <c r="N8">
+        <v>9610585</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="6"/>
+        <v>0.31805454995174537</v>
+      </c>
+      <c r="P8">
+        <v>1041956</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>28943.222222222223</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="3"/>
+        <v>30.216781999999998</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>281807</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="4"/>
+        <v>10145052</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>30000</v>
+      </c>
+      <c r="L9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="4">
+        <v>24820432</v>
+      </c>
+      <c r="N9">
+        <v>8080963</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="6"/>
+        <v>0.32557704877981175</v>
+      </c>
+      <c r="P9">
+        <v>886441</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>23327.394736842107</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="3"/>
+        <v>24.820432</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>299427</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="4"/>
+        <v>11378226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>40000</v>
+      </c>
+      <c r="L10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M10">
+        <v>42548423</v>
+      </c>
+      <c r="N10">
+        <v>12032580</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>0.28279732012629472</v>
+      </c>
+      <c r="P10">
+        <v>1467185</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>38610.131578947367</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="3"/>
+        <v>42.548423</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>394858</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="4"/>
+        <v>15004604</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>30000</v>
+      </c>
+      <c r="L11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11">
+        <v>30216782</v>
+      </c>
+      <c r="N11">
+        <v>9610585</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="6"/>
+        <v>0.31805454995174537</v>
+      </c>
+      <c r="P11">
+        <v>1041956</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>27419.894736842107</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="3"/>
+        <v>30.216781999999998</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>291322</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="4"/>
+        <v>11070236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>